<commit_message>
Add new tests adn configs.  Updated test plan
</commit_message>
<xml_diff>
--- a/documents/LFM_Test_Plan.xlsx
+++ b/documents/LFM_Test_Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LFM\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DB01E4-E3FB-4A05-8C2A-CFDF6B864C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07355EA8-FEC2-4B55-8134-3EC9FDB3E37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="199">
   <si>
     <t>Run Order</t>
   </si>
@@ -631,6 +631,9 @@
   </si>
   <si>
     <t>Vortex Quantization</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
@@ -702,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -710,6 +713,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1024,7 +1028,8 @@
     <col min="2" max="2" width="18.44140625" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
     <col min="4" max="4" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
     <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
@@ -1088,7 +1093,10 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G2" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1109,7 +1117,10 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G3" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1130,7 +1141,10 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G4" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1172,7 +1186,10 @@
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G6" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1256,7 +1273,10 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G10" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1361,7 +1381,10 @@
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G15" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1385,7 +1408,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1406,7 +1429,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1427,7 +1450,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1448,7 +1471,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1469,7 +1492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1490,7 +1513,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1508,10 +1531,13 @@
         <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+      <c r="G22" s="5">
+        <v>45953</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1532,7 +1558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1553,7 +1579,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1574,7 +1600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1595,7 +1621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1616,7 +1642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1637,7 +1663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1658,7 +1684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1679,7 +1705,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1700,7 +1726,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2056,12 +2082,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0620BAC-252D-4B86-8662-861A0B701144}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Added new tier3 energy suite tests and update plan
</commit_message>
<xml_diff>
--- a/documents/LFM_Test_Plan.xlsx
+++ b/documents/LFM_Test_Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LFM\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07355EA8-FEC2-4B55-8134-3EC9FDB3E37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814F1646-9E07-48EA-9691-7D10D364AA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiers1_3" sheetId="1" r:id="rId1"/>
@@ -1018,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1165,7 +1165,10 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G5" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1297,7 +1300,10 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G11" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1318,7 +1324,10 @@
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G12" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1339,7 +1348,10 @@
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G13" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1405,7 +1417,10 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G16" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1426,7 +1441,10 @@
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G17" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1447,7 +1465,10 @@
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G18" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1468,7 +1489,10 @@
         <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G19" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1489,7 +1513,10 @@
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G20" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1510,7 +1537,10 @@
         <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G21" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2082,7 +2112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0620BAC-252D-4B86-8662-861A0B701144}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added quantization tests and update plan
</commit_message>
<xml_diff>
--- a/documents/LFM_Test_Plan.xlsx
+++ b/documents/LFM_Test_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LFM\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814F1646-9E07-48EA-9691-7D10D364AA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919AAA1C-F4E6-4F32-B746-CC8E43F72529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="200">
   <si>
     <t>Run Order</t>
   </si>
@@ -634,6 +634,9 @@
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1022,7 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G23" sqref="G23:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1213,7 +1216,10 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G7" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1234,7 +1240,10 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G8" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1255,7 +1264,10 @@
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G9" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1372,7 +1384,10 @@
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G14" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -1585,7 +1600,10 @@
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G23" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1606,7 +1624,10 @@
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G24" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1627,7 +1648,10 @@
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G25" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1648,7 +1672,10 @@
         <v>15</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G26" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1669,7 +1696,10 @@
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G27" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1690,7 +1720,10 @@
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>16</v>
+        <v>199</v>
+      </c>
+      <c r="G28" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1711,7 +1744,10 @@
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G29" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1732,7 +1768,10 @@
         <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>16</v>
+        <v>198</v>
+      </c>
+      <c r="G30" s="5">
+        <v>45953</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fix tests, grav-10 is passing!
</commit_message>
<xml_diff>
--- a/documents/LFM_Test_Plan.xlsx
+++ b/documents/LFM_Test_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LFM\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB177A7-AAA2-46AE-9C38-B488E97DC21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85583000-42AF-4692-B1FF-8574755FA6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Tiers4_6" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tiers1_3!$A$1:$L$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tiers1_3!$A$1:$L$83</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="203">
   <si>
     <t>Run Order</t>
   </si>
@@ -123,174 +123,93 @@
     <t>REL-07</t>
   </si>
   <si>
-    <t>Polarized Wave Propagation</t>
-  </si>
-  <si>
     <t>REL-08</t>
   </si>
   <si>
-    <t>Gauge Constraint Consistency</t>
-  </si>
-  <si>
     <t>Gravity Analogue</t>
   </si>
   <si>
-    <t>GRAV-09</t>
-  </si>
-  <si>
     <t>Variable‑c Redshift — Weak Gradient</t>
   </si>
   <si>
-    <t>GRAV-10</t>
-  </si>
-  <si>
     <t>Variable‑c Redshift — Strong Gradient</t>
   </si>
   <si>
-    <t>GRAV-11</t>
-  </si>
-  <si>
     <t>Shapiro Delay — Radial</t>
   </si>
   <si>
-    <t>GRAV-12</t>
-  </si>
-  <si>
     <t>Shapiro Delay — Tangential</t>
   </si>
   <si>
-    <t>GRAV-13</t>
-  </si>
-  <si>
     <t>Weak Field Deflection</t>
   </si>
   <si>
-    <t>GRAV-14</t>
-  </si>
-  <si>
     <t>Curvature Gradient Stability</t>
   </si>
   <si>
     <t>Energy Conservation</t>
   </si>
   <si>
-    <t>ENER-15</t>
-  </si>
-  <si>
     <t>Global Conservation — Short Run</t>
   </si>
   <si>
-    <t>ENER-16</t>
-  </si>
-  <si>
     <t>Global Conservation — Long Run</t>
   </si>
   <si>
-    <t>ENER-17</t>
-  </si>
-  <si>
     <t>Wave Integrity — Mild Curvature</t>
   </si>
   <si>
-    <t>ENER-18</t>
-  </si>
-  <si>
     <t>Wave Integrity — Steep Curvature</t>
   </si>
   <si>
-    <t>ENER-19</t>
-  </si>
-  <si>
     <t>Noise‑Driven Equilibrium</t>
   </si>
   <si>
-    <t>ENER-20</t>
-  </si>
-  <si>
     <t>Thermal Mode Diffusion</t>
   </si>
   <si>
-    <t>ENER-21</t>
-  </si>
-  <si>
     <t>Entropy Growth Check</t>
   </si>
   <si>
     <t>Quantization</t>
   </si>
   <si>
-    <t>QUAN-22</t>
-  </si>
-  <si>
     <t>ΔE Transfer — Low Energy</t>
   </si>
   <si>
-    <t>QUAN-23</t>
-  </si>
-  <si>
     <t>ΔE Transfer — High Energy</t>
   </si>
   <si>
-    <t>QUAN-24</t>
-  </si>
-  <si>
     <t>Spectral Linearity — Coarse Steps</t>
   </si>
   <si>
-    <t>QUAN-25</t>
-  </si>
-  <si>
     <t>Spectral Linearity — Fine Steps</t>
   </si>
   <si>
-    <t>QUAN-26</t>
-  </si>
-  <si>
     <t>Phase‑Amplitude Coupling — Low Noise</t>
   </si>
   <si>
-    <t>QUAN-27</t>
-  </si>
-  <si>
     <t>Phase‑Amplitude Coupling — High Noise</t>
   </si>
   <si>
-    <t>QUAN-28</t>
-  </si>
-  <si>
     <t>Nonlinear Wavefront Stability</t>
   </si>
   <si>
-    <t>QUAN-29</t>
-  </si>
-  <si>
     <t>High‑Energy Lattice Blowout Test</t>
   </si>
   <si>
     <t>Quantum / Nonlocal</t>
   </si>
   <si>
-    <t>QNLC-30</t>
-  </si>
-  <si>
     <t>Entanglement Correlation — Short Distance</t>
   </si>
   <si>
-    <t>QNLC-31</t>
-  </si>
-  <si>
     <t>Entanglement Correlation — Long Distance</t>
   </si>
   <si>
-    <t>QNLC-32</t>
-  </si>
-  <si>
     <t>Entanglement — Random Phase Seeds</t>
   </si>
   <si>
-    <t>QNLC-33</t>
-  </si>
-  <si>
     <t>Decoherence Boundary Test</t>
   </si>
   <si>
@@ -634,6 +553,99 @@
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>Superposition Principle Test</t>
+  </si>
+  <si>
+    <t>REL-09</t>
+  </si>
+  <si>
+    <t>REL-10</t>
+  </si>
+  <si>
+    <t>GRAV-01</t>
+  </si>
+  <si>
+    <t>GRAV-02</t>
+  </si>
+  <si>
+    <t>GRAV-03</t>
+  </si>
+  <si>
+    <t>GRAV-04</t>
+  </si>
+  <si>
+    <t>GRAV-05</t>
+  </si>
+  <si>
+    <t>GRAV-06</t>
+  </si>
+  <si>
+    <t>ENER-01</t>
+  </si>
+  <si>
+    <t>ENER-02</t>
+  </si>
+  <si>
+    <t>ENER-03</t>
+  </si>
+  <si>
+    <t>ENER-04</t>
+  </si>
+  <si>
+    <t>ENER-05</t>
+  </si>
+  <si>
+    <t>ENER-06</t>
+  </si>
+  <si>
+    <t>ENER-07</t>
+  </si>
+  <si>
+    <t>QUAN-08</t>
+  </si>
+  <si>
+    <t>QUAN-01</t>
+  </si>
+  <si>
+    <t>QUAN-02</t>
+  </si>
+  <si>
+    <t>QUAN-03</t>
+  </si>
+  <si>
+    <t>QUAN-04</t>
+  </si>
+  <si>
+    <t>QUAN-05</t>
+  </si>
+  <si>
+    <t>QUAN-06</t>
+  </si>
+  <si>
+    <t>QUAN-07</t>
+  </si>
+  <si>
+    <t>QNLC-01</t>
+  </si>
+  <si>
+    <t>QNLC-02</t>
+  </si>
+  <si>
+    <t>QNLC-03</t>
+  </si>
+  <si>
+    <t>QNLC-04</t>
+  </si>
+  <si>
+    <t>Phase Independence Test</t>
+  </si>
+  <si>
+    <t>3D Isotropy — Directional Equivalence</t>
+  </si>
+  <si>
+    <t>3D Isotropy — Spherical Symmetry</t>
   </si>
 </sst>
 </file>
@@ -1016,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L100"/>
+  <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32:G34"/>
+      <selection activeCell="A4" sqref="A4:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1093,7 +1105,7 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G2" s="5">
         <v>45953</v>
@@ -1101,7 +1113,7 @@
     </row>
     <row r="3" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>A2+1</f>
+        <f>$A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1117,7 +1129,7 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G3" s="5">
         <v>45953</v>
@@ -1125,7 +1137,7 @@
     </row>
     <row r="4" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A34" si="0">A3+1</f>
+        <f t="shared" ref="A4:A36" si="0">$A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1141,7 +1153,7 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G4" s="5">
         <v>45953</v>
@@ -1165,7 +1177,7 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G5" s="5">
         <v>45953</v>
@@ -1189,7 +1201,7 @@
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G6" s="5">
         <v>45953</v>
@@ -1213,7 +1225,7 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G7" s="5">
         <v>45953</v>
@@ -1231,13 +1243,13 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>200</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G8" s="5">
         <v>45953</v>
@@ -1252,16 +1264,16 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>172</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G9" s="5">
         <v>45953</v>
@@ -1273,23 +1285,15 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>173</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s">
-        <v>198</v>
-      </c>
-      <c r="G10" s="5">
-        <v>45953</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -1297,23 +1301,15 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>174</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" t="s">
-        <v>198</v>
-      </c>
-      <c r="G11" s="5">
-        <v>45953</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1321,19 +1317,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>175</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G12" s="5">
         <v>45953</v>
@@ -1345,19 +1341,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>176</v>
+      </c>
+      <c r="D13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
       <c r="E13" t="s">
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G13" s="5">
         <v>45953</v>
@@ -1369,19 +1365,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>177</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G14" s="5">
         <v>45953</v>
@@ -1393,19 +1389,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>178</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G15" s="5">
         <v>45953</v>
@@ -1417,19 +1413,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>179</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G16" s="5">
         <v>45953</v>
@@ -1441,19 +1437,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>180</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G17" s="5">
         <v>45953</v>
@@ -1465,19 +1461,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>181</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G18" s="5">
         <v>45953</v>
@@ -1489,19 +1485,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>182</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G19" s="5">
         <v>45953</v>
@@ -1513,67 +1509,67 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>183</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G20" s="5">
         <v>45953</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>184</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E21" t="s">
         <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G21" s="5">
         <v>45953</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>185</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G22" s="5">
         <v>45953</v>
@@ -1585,19 +1581,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>186</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G23" s="5">
         <v>45953</v>
@@ -1609,19 +1605,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>187</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G24" s="5">
         <v>45953</v>
@@ -1633,19 +1629,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>189</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G25" s="5">
         <v>45953</v>
@@ -1657,19 +1653,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="D26" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="E26" t="s">
         <v>15</v>
       </c>
       <c r="F26" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G26" s="5">
         <v>45953</v>
@@ -1681,19 +1677,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>191</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="E27" t="s">
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G27" s="5">
         <v>45953</v>
@@ -1705,19 +1701,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>192</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G28" s="5">
         <v>45953</v>
@@ -1729,19 +1725,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>193</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G29" s="5">
         <v>45953</v>
@@ -1753,19 +1749,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>194</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G30" s="5">
         <v>45953</v>
@@ -1777,22 +1773,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>195</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G31" s="5">
-        <v>45957</v>
+        <v>45953</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1801,22 +1797,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>188</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
       </c>
       <c r="F32" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G32" s="5">
-        <v>45957</v>
+        <v>45953</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1825,19 +1821,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>196</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
       </c>
       <c r="F33" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G33" s="5">
         <v>45957</v>
@@ -1849,153 +1845,147 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>197</v>
       </c>
       <c r="D34" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
       </c>
       <c r="F34" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G34" s="5">
         <v>45957</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70">
-        <f t="shared" ref="A70:A78" si="1">A69+1</f>
-        <v>1</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>168</v>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>198</v>
+      </c>
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" t="s">
+        <v>171</v>
+      </c>
+      <c r="G35" s="5">
+        <v>45957</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" t="s">
+        <v>199</v>
+      </c>
+      <c r="D36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" t="s">
+        <v>171</v>
+      </c>
+      <c r="G36" s="5">
+        <v>45957</v>
       </c>
     </row>
     <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="3"/>
-      <c r="K72" s="3"/>
-      <c r="L72" s="3" t="s">
-        <v>171</v>
+        <f t="shared" ref="A72:A80" si="1">A71+1</f>
+        <v>1</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="4"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="4"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="F75" s="4" t="s">
         <v>16</v>
@@ -2010,19 +2000,19 @@
     <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>183</v>
+        <v>150</v>
       </c>
       <c r="F76" s="4" t="s">
         <v>16</v>
@@ -2037,19 +2027,19 @@
     <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>184</v>
+        <v>29</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="F77" s="4" t="s">
         <v>16</v>
@@ -2064,19 +2054,19 @@
     <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
       <c r="F78" s="4" t="s">
         <v>16</v>
@@ -2089,49 +2079,101 @@
       <c r="L78" s="4"/>
     </row>
     <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="2">
-        <v>78</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>193</v>
-      </c>
+      <c r="A79">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="4"/>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
     </row>
     <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="2">
-        <v>79</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>195</v>
-      </c>
+      <c r="A80">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
     </row>
     <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
+        <v>78</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="2">
+        <v>79</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2">
         <v>80</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="B83" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
     <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2149,10 +2191,12 @@
     <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="A1:L81" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L83" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2220,13 +2264,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -2241,13 +2285,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -2262,13 +2306,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -2283,13 +2327,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -2304,13 +2348,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
@@ -2325,13 +2369,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -2346,13 +2390,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
@@ -2367,13 +2411,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -2388,13 +2432,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
@@ -2409,13 +2453,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="D11" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
@@ -2430,13 +2474,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -2451,13 +2495,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
@@ -2472,13 +2516,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
@@ -2493,13 +2537,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
@@ -2514,13 +2558,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="D16" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
@@ -2535,13 +2579,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="D17" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
@@ -2556,13 +2600,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
@@ -2577,13 +2621,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="D19" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
@@ -2598,13 +2642,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="D20" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
@@ -2619,13 +2663,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="C21" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="D21" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="E21" t="s">
         <v>15</v>
@@ -2640,13 +2684,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="C22" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
@@ -2661,13 +2705,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
@@ -2682,13 +2726,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="C24" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="D24" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
@@ -2703,13 +2747,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="C25" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="D25" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -2724,16 +2768,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="C26" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="D26" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="F26" t="s">
         <v>16</v>
@@ -2745,16 +2789,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="F27" t="s">
         <v>16</v>
@@ -2766,16 +2810,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="C28" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="D28" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="E28" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="F28" t="s">
         <v>16</v>
@@ -2787,16 +2831,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="D29" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="E29" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="F29" t="s">
         <v>16</v>
@@ -2808,16 +2852,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="C30" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="D30" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="F30" t="s">
         <v>16</v>
@@ -2829,16 +2873,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="D31" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="E31" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="F31" t="s">
         <v>16</v>
@@ -2850,16 +2894,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="D32" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="E32" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="F32" t="s">
         <v>16</v>
@@ -2871,13 +2915,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>15</v>
@@ -2889,13 +2933,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>15</v>
@@ -2907,13 +2951,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>15</v>
@@ -2928,16 +2972,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Updated tests, gravity and relativity have confirmed we have a unified theory of some sort!
</commit_message>
<xml_diff>
--- a/documents/LFM_Test_Plan.xlsx
+++ b/documents/LFM_Test_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LFM\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1250B2-1E73-40D0-A9AC-1AE0B2D9CCDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1A997D-0144-4AAB-9EAE-EE68AB5C66EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tests!$A$1:$G$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tests!$A$1:$G$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
     <author>Greg Partin</author>
   </authors>
   <commentList>
-    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{30E302BC-2DA9-4E66-BF56-E9779816DA24}">
+    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{30E302BC-2DA9-4E66-BF56-E9779816DA24}">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="225">
   <si>
     <t>Run Order</t>
   </si>
@@ -701,6 +701,51 @@
   </si>
   <si>
     <t>Group Delay — Differential Timing (With vs Without Slab)</t>
+  </si>
+  <si>
+    <t>REL-11</t>
+  </si>
+  <si>
+    <t>REL-12</t>
+  </si>
+  <si>
+    <t>REL-13</t>
+  </si>
+  <si>
+    <t>REL-14</t>
+  </si>
+  <si>
+    <t>Dispersion Relation — Non-relativistic (χ/k≈10)</t>
+  </si>
+  <si>
+    <t>Dispersion Relation — Weakly Relativistic (χ/k≈1)</t>
+  </si>
+  <si>
+    <t>Dispersion Relation — Relativistic (χ/k≈0.5)</t>
+  </si>
+  <si>
+    <t>Dispersion Relation — Ultra-relativistic (χ/k≈0.1)</t>
+  </si>
+  <si>
+    <t>Shows e=mc2!</t>
+  </si>
+  <si>
+    <t>GRAV-17</t>
+  </si>
+  <si>
+    <t>Gravitational redshift — frequency shift climbing out of χ-well</t>
+  </si>
+  <si>
+    <t>GRAV-18</t>
+  </si>
+  <si>
+    <t>GRAV-19</t>
+  </si>
+  <si>
+    <t>Gravitational redshift — linear gradient (Pound-Rebka analogue)</t>
+  </si>
+  <si>
+    <t>Gravitational redshift — radial χ-profile (Schwarzschild analogue)</t>
   </si>
 </sst>
 </file>
@@ -789,7 +834,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -799,6 +844,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1101,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1184,7 +1232,7 @@
     </row>
     <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A71" si="0">$A3+1</f>
+        <f t="shared" ref="A4:A78" si="0">$A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1351,102 +1399,92 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D12" t="s">
+        <v>214</v>
+      </c>
+      <c r="E12" t="s">
+        <v>148</v>
+      </c>
+      <c r="F12" s="4">
+        <v>45960</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>211</v>
+      </c>
+      <c r="D13" t="s">
+        <v>215</v>
+      </c>
+      <c r="E13" t="s">
+        <v>148</v>
+      </c>
+      <c r="F13" s="4">
+        <v>45960</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>212</v>
+      </c>
+      <c r="D14" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" t="s">
+        <v>148</v>
+      </c>
+      <c r="F14" s="4">
+        <v>45960</v>
+      </c>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D15" t="s">
+        <v>217</v>
+      </c>
+      <c r="E15" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" s="4">
+        <v>45960</v>
+      </c>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16">
         <f>$A11+1</f>
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>152</v>
-      </c>
-      <c r="D12" t="s">
-        <v>190</v>
-      </c>
-      <c r="E12" t="s">
-        <v>148</v>
-      </c>
-      <c r="F12" s="4">
-        <v>45953</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>153</v>
-      </c>
-      <c r="D13" t="s">
-        <v>191</v>
-      </c>
-      <c r="E13" t="s">
-        <v>148</v>
-      </c>
-      <c r="F13" s="4">
-        <v>45953</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>154</v>
-      </c>
-      <c r="D14" t="s">
-        <v>192</v>
-      </c>
-      <c r="E14" t="s">
-        <v>148</v>
-      </c>
-      <c r="F14" s="4">
-        <v>45953</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D15" t="s">
-        <v>193</v>
-      </c>
-      <c r="E15" t="s">
-        <v>148</v>
-      </c>
-      <c r="F15" s="4">
-        <v>45953</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
       <c r="B16" t="s">
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E16" t="s">
         <v>148</v>
@@ -1458,16 +1496,16 @@
     <row r="17" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E17" t="s">
         <v>148</v>
@@ -1479,106 +1517,100 @@
     <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
       <c r="D18" t="s">
-        <v>205</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>186</v>
+        <v>192</v>
+      </c>
+      <c r="E18" t="s">
+        <v>148</v>
       </c>
       <c r="F18" s="4">
-        <v>45959</v>
-      </c>
-      <c r="G18" t="s">
-        <v>189</v>
+        <v>45953</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="D19" t="s">
-        <v>196</v>
-      </c>
-      <c r="E19" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E19" t="s">
         <v>148</v>
       </c>
       <c r="F19" s="4">
-        <v>45959</v>
-      </c>
-      <c r="G19" t="s">
-        <v>187</v>
+        <v>45953</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="D20" t="s">
-        <v>206</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>186</v>
+        <v>194</v>
+      </c>
+      <c r="E20" t="s">
+        <v>148</v>
       </c>
       <c r="F20" s="4">
-        <v>45959</v>
+        <v>45953</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="D21" t="s">
-        <v>207</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>186</v>
+        <v>195</v>
+      </c>
+      <c r="E21" t="s">
+        <v>148</v>
       </c>
       <c r="F21" s="4">
-        <v>45959</v>
+        <v>45953</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>185</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>208</v>
+        <v>181</v>
+      </c>
+      <c r="D22" t="s">
+        <v>205</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>186</v>
@@ -1586,20 +1618,23 @@
       <c r="F22" s="4">
         <v>45959</v>
       </c>
+      <c r="G22" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>204</v>
+      <c r="C23" t="s">
+        <v>182</v>
+      </c>
+      <c r="D23" t="s">
+        <v>196</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>148</v>
@@ -1607,23 +1642,26 @@
       <c r="F23" s="4">
         <v>45959</v>
       </c>
+      <c r="G23" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>197</v>
+      <c r="C24" t="s">
+        <v>183</v>
+      </c>
+      <c r="D24" t="s">
+        <v>206</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="F24" s="4">
         <v>45959</v>
@@ -1632,16 +1670,16 @@
     <row r="25" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>209</v>
+      <c r="C25" t="s">
+        <v>184</v>
+      </c>
+      <c r="D25" t="s">
+        <v>207</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>186</v>
@@ -1653,19 +1691,19 @@
     <row r="26" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>199</v>
+      <c r="C26" t="s">
+        <v>185</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="F26" s="4">
         <v>45959</v>
@@ -1674,16 +1712,16 @@
     <row r="27" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>148</v>
@@ -1695,282 +1733,310 @@
     <row r="28" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" t="s">
-        <v>158</v>
-      </c>
-      <c r="D28" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F28" s="4">
+        <v>45959</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" t="s">
-        <v>159</v>
-      </c>
-      <c r="D29" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F29" s="4">
+        <v>45959</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" t="s">
-        <v>160</v>
-      </c>
-      <c r="D30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" s="4">
+        <v>45959</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" t="s">
-        <v>161</v>
-      </c>
-      <c r="D31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F31" s="4">
+        <v>45959</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F32" s="4">
+        <v>45960</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F33" s="4">
+        <v>45960</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F34" s="4">
+        <v>45960</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" t="s">
+        <v>148</v>
+      </c>
+      <c r="F35" s="4">
+        <v>45960</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B36" t="s">
         <v>24</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C36" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" t="s">
+        <v>148</v>
+      </c>
+      <c r="F36" s="4">
+        <v>45960</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" t="s">
+        <v>148</v>
+      </c>
+      <c r="F37" s="4">
+        <v>45960</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" t="s">
+        <v>148</v>
+      </c>
+      <c r="F38" s="4">
+        <v>45960</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" t="s">
         <v>162</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D39" t="s">
         <v>29</v>
       </c>
-      <c r="E32" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" t="s">
-        <v>163</v>
-      </c>
-      <c r="D33" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" t="s">
-        <v>164</v>
-      </c>
-      <c r="D34" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" t="s">
-        <v>166</v>
-      </c>
-      <c r="D35" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" t="s">
-        <v>167</v>
-      </c>
-      <c r="D36" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" t="s">
-        <v>168</v>
-      </c>
-      <c r="D37" t="s">
-        <v>35</v>
-      </c>
-      <c r="E37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" t="s">
-        <v>169</v>
-      </c>
-      <c r="D38" t="s">
-        <v>36</v>
-      </c>
-      <c r="E38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" t="s">
-        <v>170</v>
-      </c>
-      <c r="D39" t="s">
-        <v>37</v>
-      </c>
       <c r="E39" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="4"/>
+        <v>148</v>
+      </c>
+      <c r="F39" s="4">
+        <v>45960</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D40" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="4"/>
+        <v>148</v>
+      </c>
+      <c r="F40" s="4">
+        <v>45960</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D41" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="4"/>
+        <v>148</v>
+      </c>
+      <c r="F41" s="4">
+        <v>45960</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B42" t="s">
         <v>32</v>
       </c>
       <c r="C42" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D42" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1980,16 +2046,16 @@
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C43" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -1999,16 +2065,16 @@
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C44" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D44" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
@@ -2018,16 +2084,16 @@
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C45" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D45" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E45" t="s">
         <v>10</v>
@@ -2037,341 +2103,348 @@
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" t="s">
+        <v>171</v>
+      </c>
+      <c r="D47" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" t="s">
+        <v>172</v>
+      </c>
+      <c r="D48" t="s">
+        <v>39</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" t="s">
+        <v>165</v>
+      </c>
+      <c r="D49" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B50" t="s">
         <v>41</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C50" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" t="s">
+        <v>174</v>
+      </c>
+      <c r="D51" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" t="s">
+        <v>175</v>
+      </c>
+      <c r="D52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" t="s">
         <v>176</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D53" t="s">
         <v>45</v>
       </c>
-      <c r="E46" t="s">
-        <v>10</v>
-      </c>
-      <c r="F46" s="4"/>
-    </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <f t="shared" si="0"/>
+      <c r="E53" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B54" t="s">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C54" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B55" t="s">
         <v>46</v>
       </c>
-      <c r="C47" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" t="s">
-        <v>48</v>
-      </c>
-      <c r="E47" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="C55" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55" t="s">
+        <v>50</v>
+      </c>
+      <c r="E55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B56" t="s">
         <v>46</v>
       </c>
-      <c r="C48" t="s">
-        <v>49</v>
-      </c>
-      <c r="D48" t="s">
-        <v>50</v>
-      </c>
-      <c r="E48" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D56" t="s">
+        <v>52</v>
+      </c>
+      <c r="E56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B57" t="s">
         <v>46</v>
       </c>
-      <c r="C49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D49" t="s">
-        <v>52</v>
-      </c>
-      <c r="E49" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="C57" t="s">
         <v>53</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D57" t="s">
         <v>54</v>
       </c>
-      <c r="E50" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>55</v>
-      </c>
-      <c r="C51" t="s">
-        <v>56</v>
-      </c>
-      <c r="D51" t="s">
-        <v>57</v>
-      </c>
-      <c r="E51" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" t="s">
-        <v>58</v>
-      </c>
-      <c r="D52" t="s">
-        <v>59</v>
-      </c>
-      <c r="E52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>55</v>
-      </c>
-      <c r="C53" t="s">
-        <v>60</v>
-      </c>
-      <c r="D53" t="s">
-        <v>61</v>
-      </c>
-      <c r="E53" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54">
+      <c r="E57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58">
         <f t="shared" si="0"/>
         <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>55</v>
-      </c>
-      <c r="C54" t="s">
-        <v>62</v>
-      </c>
-      <c r="D54" t="s">
-        <v>63</v>
-      </c>
-      <c r="E54" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>55</v>
-      </c>
-      <c r="C55" t="s">
-        <v>64</v>
-      </c>
-      <c r="D55" t="s">
-        <v>65</v>
-      </c>
-      <c r="E55" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B56" t="s">
-        <v>55</v>
-      </c>
-      <c r="C56" t="s">
-        <v>66</v>
-      </c>
-      <c r="D56" t="s">
-        <v>67</v>
-      </c>
-      <c r="E56" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B57" t="s">
-        <v>55</v>
-      </c>
-      <c r="C57" t="s">
-        <v>68</v>
-      </c>
-      <c r="D57" t="s">
-        <v>69</v>
-      </c>
-      <c r="E57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <f t="shared" si="0"/>
-        <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>55</v>
       </c>
       <c r="C58" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D58" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="E58" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B59" t="s">
         <v>55</v>
       </c>
       <c r="C59" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D59" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E59" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B60" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B61" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" t="s">
+        <v>63</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B62" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62" t="s">
+        <v>65</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B63" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" t="s">
+        <v>66</v>
+      </c>
+      <c r="D63" t="s">
+        <v>67</v>
+      </c>
+      <c r="E63" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B60" t="s">
-        <v>74</v>
-      </c>
-      <c r="C60" t="s">
-        <v>75</v>
-      </c>
-      <c r="D60" t="s">
-        <v>76</v>
-      </c>
-      <c r="E60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B61" t="s">
-        <v>74</v>
-      </c>
-      <c r="C61" t="s">
-        <v>77</v>
-      </c>
-      <c r="D61" t="s">
-        <v>78</v>
-      </c>
-      <c r="E61" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B62" t="s">
-        <v>74</v>
-      </c>
-      <c r="C62" t="s">
-        <v>79</v>
-      </c>
-      <c r="D62" t="s">
-        <v>80</v>
-      </c>
-      <c r="E62" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B63" t="s">
-        <v>74</v>
-      </c>
-      <c r="C63" t="s">
-        <v>81</v>
-      </c>
-      <c r="D63" t="s">
-        <v>82</v>
-      </c>
-      <c r="E63" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C64" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D64" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E64" t="s">
         <v>10</v>
@@ -2380,16 +2453,16 @@
     <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B65" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C65" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D65" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="E65" t="s">
         <v>10</v>
@@ -2398,16 +2471,16 @@
     <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C66" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D66" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E66" t="s">
         <v>10</v>
@@ -2416,16 +2489,16 @@
     <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" si="0"/>
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C67" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="D67" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E67" t="s">
         <v>10</v>
@@ -2434,16 +2507,16 @@
     <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B68" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C68" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="D68" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="E68" t="s">
         <v>10</v>
@@ -2452,16 +2525,16 @@
     <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C69" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="D69" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E69" t="s">
         <v>10</v>
@@ -2470,16 +2543,16 @@
     <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B70" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C70" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D70" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E70" t="s">
         <v>10</v>
@@ -2488,16 +2561,16 @@
     <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B71" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C71" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D71" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="E71" t="s">
         <v>10</v>
@@ -2505,17 +2578,17 @@
     </row>
     <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72">
-        <f t="shared" ref="A72:A92" si="1">$A71+1</f>
-        <v>71</v>
+        <f t="shared" si="0"/>
+        <v>67</v>
       </c>
       <c r="B72" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C72" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D72" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="E72" t="s">
         <v>10</v>
@@ -2523,17 +2596,17 @@
     </row>
     <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73">
-        <f t="shared" si="1"/>
-        <v>72</v>
+        <f t="shared" si="0"/>
+        <v>68</v>
       </c>
       <c r="B73" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C73" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="D73" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="E73" t="s">
         <v>10</v>
@@ -2541,17 +2614,17 @@
     </row>
     <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74">
-        <f t="shared" si="1"/>
-        <v>73</v>
+        <f t="shared" si="0"/>
+        <v>69</v>
       </c>
       <c r="B74" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C74" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="D74" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E74" t="s">
         <v>10</v>
@@ -2559,17 +2632,17 @@
     </row>
     <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75">
-        <f t="shared" si="1"/>
-        <v>74</v>
+        <f t="shared" si="0"/>
+        <v>70</v>
       </c>
       <c r="B75" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C75" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="D75" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="E75" t="s">
         <v>10</v>
@@ -2577,17 +2650,17 @@
     </row>
     <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76">
-        <f t="shared" si="1"/>
-        <v>75</v>
+        <f t="shared" si="0"/>
+        <v>71</v>
       </c>
       <c r="B76" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C76" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="D76" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="E76" t="s">
         <v>10</v>
@@ -2595,17 +2668,17 @@
     </row>
     <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77">
-        <f t="shared" si="1"/>
-        <v>76</v>
+        <f t="shared" si="0"/>
+        <v>72</v>
       </c>
       <c r="B77" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C77" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="D77" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="E77" t="s">
         <v>10</v>
@@ -2613,17 +2686,17 @@
     </row>
     <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78">
-        <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>116</v>
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="B78" t="s">
+        <v>98</v>
+      </c>
+      <c r="C78" t="s">
+        <v>99</v>
+      </c>
+      <c r="D78" t="s">
+        <v>100</v>
       </c>
       <c r="E78" t="s">
         <v>10</v>
@@ -2631,17 +2704,17 @@
     </row>
     <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>118</v>
+        <f t="shared" ref="A79:A99" si="1">$A78+1</f>
+        <v>74</v>
+      </c>
+      <c r="B79" t="s">
+        <v>98</v>
+      </c>
+      <c r="C79" t="s">
+        <v>101</v>
+      </c>
+      <c r="D79" t="s">
+        <v>102</v>
       </c>
       <c r="E79" t="s">
         <v>10</v>
@@ -2650,16 +2723,16 @@
     <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>120</v>
+        <v>75</v>
+      </c>
+      <c r="B80" t="s">
+        <v>98</v>
+      </c>
+      <c r="C80" t="s">
+        <v>103</v>
+      </c>
+      <c r="D80" t="s">
+        <v>104</v>
       </c>
       <c r="E80" t="s">
         <v>10</v>
@@ -2668,190 +2741,178 @@
     <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>122</v>
+        <v>76</v>
+      </c>
+      <c r="B81" t="s">
+        <v>98</v>
+      </c>
+      <c r="C81" t="s">
+        <v>105</v>
+      </c>
+      <c r="D81" t="s">
+        <v>106</v>
       </c>
       <c r="E81" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82">
         <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>125</v>
+        <v>77</v>
+      </c>
+      <c r="B82" t="s">
+        <v>107</v>
+      </c>
+      <c r="C82" t="s">
+        <v>108</v>
+      </c>
+      <c r="D82" t="s">
+        <v>109</v>
       </c>
       <c r="E82" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>127</v>
+        <v>78</v>
+      </c>
+      <c r="B83" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" t="s">
+        <v>110</v>
+      </c>
+      <c r="D83" t="s">
+        <v>111</v>
       </c>
       <c r="E83" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>129</v>
+        <v>79</v>
+      </c>
+      <c r="B84" t="s">
+        <v>107</v>
+      </c>
+      <c r="C84" t="s">
+        <v>112</v>
+      </c>
+      <c r="D84" t="s">
+        <v>113</v>
       </c>
       <c r="E84" t="s">
         <v>10</v>
       </c>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
-    </row>
-    <row r="85" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>131</v>
+        <v>80</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="E85" t="s">
         <v>10</v>
       </c>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
-    </row>
-    <row r="86" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>133</v>
+        <v>81</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="E86" t="s">
         <v>10</v>
       </c>
-      <c r="F86" s="3"/>
-      <c r="G86" s="3"/>
-    </row>
-    <row r="87" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>135</v>
+        <v>82</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="E87" t="s">
         <v>10</v>
       </c>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
-    </row>
-    <row r="88" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88">
         <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>138</v>
+        <v>83</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="E88" t="s">
         <v>10</v>
       </c>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
     </row>
     <row r="89" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89">
         <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>140</v>
+        <v>84</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="E89" t="s">
         <v>10</v>
       </c>
-      <c r="F89" s="3"/>
-      <c r="G89" s="3"/>
     </row>
     <row r="90" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>143</v>
+        <v>123</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="E90" t="s">
         <v>10</v>
@@ -2860,60 +2921,201 @@
     <row r="91" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>141</v>
+        <v>86</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="E91" t="s">
         <v>10</v>
       </c>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
     </row>
     <row r="92" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92">
         <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E92" t="s">
+        <v>10</v>
+      </c>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+    </row>
+    <row r="93" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E93" t="s">
+        <v>10</v>
+      </c>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+    </row>
+    <row r="94" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E94" t="s">
+        <v>10</v>
+      </c>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+    </row>
+    <row r="95" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E95" t="s">
+        <v>10</v>
+      </c>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+    </row>
+    <row r="96" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B96" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E96" t="s">
+        <v>10</v>
+      </c>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+    </row>
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="C97" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E97" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E98" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C99" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D99" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E92" s="2" t="s">
+      <c r="E99" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="A1:G92" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G99" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <mergeCells count="1">
+    <mergeCell ref="G12:G15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Forgot to mark as passed!
</commit_message>
<xml_diff>
--- a/documents/LFM_Test_Plan.xlsx
+++ b/documents/LFM_Test_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LFM\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1A997D-0144-4AAB-9EAE-EE68AB5C66EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FD47A3-7853-4056-836C-6DA4DD50E0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1152,7 +1152,7 @@
   <dimension ref="A1:G118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1850,7 +1850,7 @@
         <v>223</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="F33" s="4">
         <v>45960</v>

</xml_diff>